<commit_message>
Se arreglo la carga masiva de asistentes.
</commit_message>
<xml_diff>
--- a/app/assets/data/attendees_template.xlsx
+++ b/app/assets/data/attendees_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="146" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="82" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>REGISTRATION ID</t>
   </si>
@@ -104,6 +104,12 @@
     <t>MARKET SEGMENT</t>
   </si>
   <si>
+    <t>SECTOR</t>
+  </si>
+  <si>
+    <t>WANT TO RECEIVE EMAIL?</t>
+  </si>
+  <si>
     <t>EV0001</t>
   </si>
   <si>
@@ -146,19 +152,22 @@
     <t>Android;IPhone</t>
   </si>
   <si>
-    <t>Aplicaciones Web</t>
-  </si>
-  <si>
-    <t>Capacitación</t>
-  </si>
-  <si>
-    <t>Desarrollo</t>
+    <t>Web applications</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Development</t>
   </si>
   <si>
     <t>http://emobile.com.mx</t>
   </si>
   <si>
     <t>Gobierno;Corporativo;Web;PyMEs</t>
+  </si>
+  <si>
+    <t>Public</t>
   </si>
   <si>
     <t>Note: Red columns are mandatory and platforms and market segments must be separated by semicolons.</t>
@@ -171,7 +180,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -204,6 +213,7 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -211,7 +221,14 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFDC2300"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -266,7 +283,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -287,6 +304,10 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -296,6 +317,66 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFDC2300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -304,10 +385,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC23"/>
+  <dimension ref="A1:AE23"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A24" activeCellId="0" pane="topLeft" sqref="A24"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="U1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="Z1" activeCellId="0" pane="topLeft" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -338,8 +419,10 @@
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="24.4948979591837"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.5459183673469"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="20.5612244897959"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="39.9234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="32.9285714285714"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="28.3367346938776"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="29.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="32" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -352,7 +435,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -361,7 +444,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -379,7 +462,7 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -394,82 +477,88 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>4709</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>31105</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>614</v>
@@ -478,13 +567,13 @@
         <v>4191895</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="S2" s="0" t="n">
         <v>6141111111</v>
@@ -496,33 +585,39 @@
         <v>53</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Z2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se hicieron modificaciones en la carga masiva .
</commit_message>
<xml_diff>
--- a/app/assets/data/attendees_template.xlsx
+++ b/app/assets/data/attendees_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>REGISTRATION ID</t>
   </si>
@@ -110,6 +110,9 @@
     <t>WANT TO RECEIVE EMAIL?</t>
   </si>
   <si>
+    <t>JOB</t>
+  </si>
+  <si>
     <t>EV0001</t>
   </si>
   <si>
@@ -168,6 +171,9 @@
   </si>
   <si>
     <t>Public</t>
+  </si>
+  <si>
+    <t>Selling</t>
   </si>
   <si>
     <t>Note: Red columns are mandatory and platforms and market segments must be separated by semicolons.</t>
@@ -385,10 +391,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE23"/>
+  <dimension ref="A1:AF23"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="U1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="Z1" activeCellId="0" pane="topLeft" sqref="Z1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="Z1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="AF2" activeCellId="0" pane="topLeft" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -519,46 +525,49 @@
       <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="AF1" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>4709</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>31105</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>614</v>
@@ -567,13 +576,13 @@
         <v>4191895</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S2" s="0" t="n">
         <v>6141111111</v>
@@ -585,39 +594,42 @@
         <v>53</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Z2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>